<commit_message>
Avance servidor pool 25-04 Casa
</commit_message>
<xml_diff>
--- a/spotify/bbdd-songs.xlsx
+++ b/spotify/bbdd-songs.xlsx
@@ -1,23 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\cursoFullStack\spotify\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaco\Documents\Learning\Code\Curso Full Stack Tu Carrera Digital\cursoFullStack\spotify\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{282C411F-4FD6-406F-8F8E-55B86849CE3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9264"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -515,7 +524,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -878,24 +887,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:M77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4:K53"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K30" sqref="K30:K53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="16.88671875" customWidth="1"/>
-    <col min="5" max="5" width="16.77734375" customWidth="1"/>
-    <col min="6" max="6" width="5.109375" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" customWidth="1"/>
+    <col min="6" max="6" width="5.140625" customWidth="1"/>
     <col min="7" max="7" width="5" customWidth="1"/>
-    <col min="8" max="8" width="6.44140625" customWidth="1"/>
-    <col min="11" max="11" width="88.33203125" customWidth="1"/>
+    <col min="8" max="8" width="6.42578125" customWidth="1"/>
+    <col min="11" max="11" width="88.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.25">
       <c r="C3" s="5" t="s">
         <v>55</v>
       </c>
@@ -924,7 +933,7 @@
       <c r="L3" s="5"/>
       <c r="M3" s="5"/>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B4" t="str">
         <f>CONCATENATE(C4,D4)</f>
         <v>https://www.parkwaycleanersorl.com/music/daddy-yankee/king-daddy/la-rompe-carros.mp3</v>
@@ -955,7 +964,7 @@
         <v>INSERT INTO `song` (`id`, `song_name`, `artist_id`, `album_id`, `song_description`, `song_length`, `song_url`) VALUES (NULL,'La Rompe Carros','3','7','','0','https://www.parkwaycleanersorl.com/music/daddy-yankee/king-daddy/la-rompe-carros.mp3');</v>
       </c>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B5" t="str">
         <f t="shared" ref="B5:B53" si="0">CONCATENATE(C5,D5)</f>
         <v>https://www.parkwaycleanersorl.com/music/daddy-yankee/king-daddy/donde-es-el-party.mp3</v>
@@ -986,7 +995,7 @@
         <v>INSERT INTO `song` (`id`, `song_name`, `artist_id`, `album_id`, `song_description`, `song_length`, `song_url`) VALUES (NULL,'Donde Es El Party','3','7','','0','https://www.parkwaycleanersorl.com/music/daddy-yankee/king-daddy/donde-es-el-party.mp3');</v>
       </c>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B6" t="str">
         <f t="shared" si="0"/>
         <v>https://www.parkwaycleanersorl.com/music/daddy-yankee/king-daddy/im-the-boss.mp3</v>
@@ -1017,7 +1026,7 @@
         <v>INSERT INTO `song` (`id`, `song_name`, `artist_id`, `album_id`, `song_description`, `song_length`, `song_url`) VALUES (NULL,'Im The Boss','3','7','','0','https://www.parkwaycleanersorl.com/music/daddy-yankee/king-daddy/im-the-boss.mp3');</v>
       </c>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B7" t="str">
         <f t="shared" si="0"/>
         <v>https://www.parkwaycleanersorl.com/music/daddy-yankee/king-daddy/la-nueva-y-la-ex.mp3</v>
@@ -1048,7 +1057,7 @@
         <v>INSERT INTO `song` (`id`, `song_name`, `artist_id`, `album_id`, `song_description`, `song_length`, `song_url`) VALUES (NULL,'La Nueva Y La Ex','3','7','','0','https://www.parkwaycleanersorl.com/music/daddy-yankee/king-daddy/la-nueva-y-la-ex.mp3');</v>
       </c>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B8" t="str">
         <f t="shared" si="0"/>
         <v>https://www.parkwaycleanersorl.com/music/daddy-yankee/king-daddy/mil-problemas.mp3</v>
@@ -1079,7 +1088,7 @@
         <v>INSERT INTO `song` (`id`, `song_name`, `artist_id`, `album_id`, `song_description`, `song_length`, `song_url`) VALUES (NULL,'Mil Problemas','3','7','','0','https://www.parkwaycleanersorl.com/music/daddy-yankee/king-daddy/mil-problemas.mp3');</v>
       </c>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B9" t="str">
         <f t="shared" si="0"/>
         <v>https://www.parkwaycleanersorl.com/music/daddy-yankee/king-daddy/millonarios.mp3</v>
@@ -1110,7 +1119,7 @@
         <v>INSERT INTO `song` (`id`, `song_name`, `artist_id`, `album_id`, `song_description`, `song_length`, `song_url`) VALUES (NULL,'Millonarios','3','7','','0','https://www.parkwaycleanersorl.com/music/daddy-yankee/king-daddy/millonarios.mp3');</v>
       </c>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B10" t="str">
         <f t="shared" si="0"/>
         <v>https://www.parkwaycleanersorl.com/music/daddy-yankee/king-daddy/nada-ha-cambiado.mp3</v>
@@ -1141,7 +1150,7 @@
         <v>INSERT INTO `song` (`id`, `song_name`, `artist_id`, `album_id`, `song_description`, `song_length`, `song_url`) VALUES (NULL,'Nada Ha Cambiado','3','7','','0','https://www.parkwaycleanersorl.com/music/daddy-yankee/king-daddy/nada-ha-cambiado.mp3');</v>
       </c>
     </row>
-    <row r="11" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B11" t="str">
         <f t="shared" si="0"/>
         <v>https://www.parkwaycleanersorl.com/music/daddy-yankee/king-daddy/suena-boom.mp3</v>
@@ -1172,7 +1181,7 @@
         <v>INSERT INTO `song` (`id`, `song_name`, `artist_id`, `album_id`, `song_description`, `song_length`, `song_url`) VALUES (NULL,'Suena Boom','3','7','','0','https://www.parkwaycleanersorl.com/music/daddy-yankee/king-daddy/suena-boom.mp3');</v>
       </c>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B12" t="str">
         <f t="shared" si="0"/>
         <v>https://www.parkwaycleanersorl.com/music/daddy-yankee/king-daddy/una-respuesta.mp3</v>
@@ -1203,7 +1212,7 @@
         <v>INSERT INTO `song` (`id`, `song_name`, `artist_id`, `album_id`, `song_description`, `song_length`, `song_url`) VALUES (NULL,'Una Respuesta','3','7','','0','https://www.parkwaycleanersorl.com/music/daddy-yankee/king-daddy/una-respuesta.mp3');</v>
       </c>
     </row>
-    <row r="13" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B13" t="str">
         <f t="shared" si="0"/>
         <v>https://www.parkwaycleanersorl.com/music/daddy-yankee/king-daddy/calenton.mp3</v>
@@ -1234,7 +1243,7 @@
         <v>INSERT INTO `song` (`id`, `song_name`, `artist_id`, `album_id`, `song_description`, `song_length`, `song_url`) VALUES (NULL,'Calenton','3','7','','0','https://www.parkwaycleanersorl.com/music/daddy-yankee/king-daddy/calenton.mp3');</v>
       </c>
     </row>
-    <row r="14" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B14" t="str">
         <f t="shared" si="0"/>
         <v>https://www.parkwaycleanersorl.com/music/daddy-yankee/king-daddy/dejala-caer.mp3</v>
@@ -1265,7 +1274,7 @@
         <v>INSERT INTO `song` (`id`, `song_name`, `artist_id`, `album_id`, `song_description`, `song_length`, `song_url`) VALUES (NULL,'Dejala Caer','3','7','','0','https://www.parkwaycleanersorl.com/music/daddy-yankee/king-daddy/dejala-caer.mp3');</v>
       </c>
     </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B15" t="str">
         <f t="shared" si="0"/>
         <v>https://www.parkwaycleanersorl.com/music/maria-becerra/animal/J Balvin, Maria Becerra - Qué Más Pues (Official Video).mp3</v>
@@ -1296,7 +1305,7 @@
         <v>INSERT INTO `song` (`id`, `song_name`, `artist_id`, `album_id`, `song_description`, `song_length`, `song_url`) VALUES (NULL,'Qué Más Pues','3','7','','0','https://www.parkwaycleanersorl.com/music/maria-becerra/animal/J%Balvin,%Maria%Becerra%-%Qué%Más%Pues%(Official%Video).mp3');</v>
       </c>
     </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B16" t="str">
         <f t="shared" si="0"/>
         <v>https://www.parkwaycleanersorl.com/music/maria-becerra/animal/Maria Becerra - A SOLAS (Official Video).mp3</v>
@@ -1327,7 +1336,7 @@
         <v>INSERT INTO `song` (`id`, `song_name`, `artist_id`, `album_id`, `song_description`, `song_length`, `song_url`) VALUES (NULL,'A Solas','1','6','','0','https://www.parkwaycleanersorl.com/music/maria-becerra/animal/Maria%Becerra%-%A%SOLAS%(Official%Video).mp3');</v>
       </c>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" t="str">
         <f t="shared" si="0"/>
         <v>https://www.parkwaycleanersorl.com/music/maria-becerra/animal/Maria Becerra - ACARAMELAO (Official Video).mp3</v>
@@ -1358,7 +1367,7 @@
         <v>INSERT INTO `song` (`id`, `song_name`, `artist_id`, `album_id`, `song_description`, `song_length`, `song_url`) VALUES (NULL,'Acaramelao','1','6','','0','https://www.parkwaycleanersorl.com/music/maria-becerra/animal/Maria%Becerra%-%ACARAMELAO%(Official%Video).mp3');</v>
       </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18" t="str">
         <f t="shared" si="0"/>
         <v>https://www.parkwaycleanersorl.com/music/maria-becerra/animal/Maria Becerra - CERQUITA DE TI (Official Video).mp3</v>
@@ -1389,7 +1398,7 @@
         <v>INSERT INTO `song` (`id`, `song_name`, `artist_id`, `album_id`, `song_description`, `song_length`, `song_url`) VALUES (NULL,'Cerquita De Ti','1','6','','0','https://www.parkwaycleanersorl.com/music/maria-becerra/animal/Maria%Becerra%-%CERQUITA%DE%TI%(Official%Video).mp3');</v>
       </c>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" t="str">
         <f t="shared" si="0"/>
         <v>https://www.parkwaycleanersorl.com/music/maria-becerra/animal/Maria Becerra - Episodios (Official Lyric Video).mp3</v>
@@ -1420,7 +1429,7 @@
         <v>INSERT INTO `song` (`id`, `song_name`, `artist_id`, `album_id`, `song_description`, `song_length`, `song_url`) VALUES (NULL,'Episodios','1','6','','0','https://www.parkwaycleanersorl.com/music/maria-becerra/animal/Maria%Becerra%-%Episodios%(Official%Lyric%Video).mp3');</v>
       </c>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B20" t="str">
         <f t="shared" si="0"/>
         <v>https://www.parkwaycleanersorl.com/music/maria-becerra/animal/Maria Becerra - Hace Rato (Official Lyric Video).mp3</v>
@@ -1451,7 +1460,7 @@
         <v>INSERT INTO `song` (`id`, `song_name`, `artist_id`, `album_id`, `song_description`, `song_length`, `song_url`) VALUES (NULL,'Hace Rato','1','6','','0','https://www.parkwaycleanersorl.com/music/maria-becerra/animal/Maria%Becerra%-%Hace%Rato%(Official%Lyric%Video).mp3');</v>
       </c>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B21" t="str">
         <f t="shared" si="0"/>
         <v>https://www.parkwaycleanersorl.com/music/maria-becerra/animal/Maria Becerra - Hipnotiza' (Official Lyric Video).mp3</v>
@@ -1482,7 +1491,7 @@
         <v>INSERT INTO `song` (`id`, `song_name`, `artist_id`, `album_id`, `song_description`, `song_length`, `song_url`) VALUES (NULL,'Hipnotiza','1','6','','0','https://www.parkwaycleanersorl.com/music/maria-becerra/animal/Maria%Becerra%-%Hipnotiza'%(Official%Lyric%Video).mp3');</v>
       </c>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B22" t="str">
         <f t="shared" si="0"/>
         <v>https://www.parkwaycleanersorl.com/music/maria-becerra/animal/Maria Becerra - MI DEBILIDAD (Official Video).mp3</v>
@@ -1513,7 +1522,7 @@
         <v>INSERT INTO `song` (`id`, `song_name`, `artist_id`, `album_id`, `song_description`, `song_length`, `song_url`) VALUES (NULL,'Mi Debilidad','1','6','','0','https://www.parkwaycleanersorl.com/music/maria-becerra/animal/Maria%Becerra%-%MI%DEBILIDAD%(Official%Video).mp3');</v>
       </c>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B23" t="str">
         <f t="shared" si="0"/>
         <v>https://www.parkwaycleanersorl.com/music/maria-becerra/animal/Maria Becerra x TINI x Lola Indigo - High Remix (Official Video).mp3</v>
@@ -1544,7 +1553,7 @@
         <v>INSERT INTO `song` (`id`, `song_name`, `artist_id`, `album_id`, `song_description`, `song_length`, `song_url`) VALUES (NULL,'High Remix','1','6','','0','https://www.parkwaycleanersorl.com/music/maria-becerra/animal/Maria%Becerra%x%TINI%x%Lola%Indigo%-%High%Remix%(Official%Video).mp3');</v>
       </c>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B24" t="str">
         <f t="shared" si="0"/>
         <v>https://www.parkwaycleanersorl.com/music/maria-becerra/animal/Maria Becerra, Becky G - WOW WOW (Official Video).mp3</v>
@@ -1576,7 +1585,7 @@
         <v>INSERT INTO `song` (`id`, `song_name`, `artist_id`, `album_id`, `song_description`, `song_length`, `song_url`) VALUES (NULL,'Wow Wow','1','6','','0','https://www.parkwaycleanersorl.com/music/maria-becerra/animal/Maria%Becerra,%Becky%G%-%WOW%WOW%(Official%Video).mp3');</v>
       </c>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B25" t="str">
         <f t="shared" si="0"/>
         <v>https://www.parkwaycleanersorl.com/music/maria-becerra/animal/Maria Becerra, Cazzu - ANIMAL (Official Video).mp3</v>
@@ -1608,7 +1617,7 @@
         <v>INSERT INTO `song` (`id`, `song_name`, `artist_id`, `album_id`, `song_description`, `song_length`, `song_url`) VALUES (NULL,'Animal','1','6','','0','https://www.parkwaycleanersorl.com/music/maria-becerra/animal/Maria%Becerra,%Cazzu%-%ANIMAL%(Official%Video).mp3');</v>
       </c>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B26" t="str">
         <f t="shared" si="0"/>
         <v>https://www.parkwaycleanersorl.com/music/maria-becerra/animal/Maria Becerra, Danny Ocean - No Eres Tu Soy Yo (Official Video).mp3</v>
@@ -1640,7 +1649,7 @@
         <v>INSERT INTO `song` (`id`, `song_name`, `artist_id`, `album_id`, `song_description`, `song_length`, `song_url`) VALUES (NULL,'No Eres Tu Soy Yo','1','6','','0','https://www.parkwaycleanersorl.com/music/maria-becerra/animal/Maria%Becerra,%Danny%Ocean%-%No%Eres%Tu%Soy%Yo%(Official%Video).mp3');</v>
       </c>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B27" t="str">
         <f t="shared" si="0"/>
         <v>https://www.parkwaycleanersorl.com/music/maria-becerra/animal/Maria Becerra, RusherKing - Confiésalo (Official Video).mp3</v>
@@ -1672,7 +1681,7 @@
         <v>INSERT INTO `song` (`id`, `song_name`, `artist_id`, `album_id`, `song_description`, `song_length`, `song_url`) VALUES (NULL,'Confiésalo','1','6','','0','https://www.parkwaycleanersorl.com/music/maria-becerra/animal/Maria%Becerra,%RusherKing%-%Confiésalo%(Official%Video).mp3');</v>
       </c>
     </row>
-    <row r="28" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B28" t="str">
         <f t="shared" si="0"/>
         <v>https://www.parkwaycleanersorl.com/music/maria-becerra/animal/Maria Becerra, Tiago PZK - CAZAME (Official Video).mp3</v>
@@ -1704,7 +1713,7 @@
         <v>INSERT INTO `song` (`id`, `song_name`, `artist_id`, `album_id`, `song_description`, `song_length`, `song_url`) VALUES (NULL,'Cazame','1','6','','0','https://www.parkwaycleanersorl.com/music/maria-becerra/animal/Maria%Becerra,%Tiago%PZK%-%CAZAME%(Official%Video).mp3');</v>
       </c>
     </row>
-    <row r="29" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B29" t="str">
         <f t="shared" si="0"/>
         <v>https://www.parkwaycleanersorl.com/music/ozuna/enoc/Caramelo (Remix).mp3</v>
@@ -1736,7 +1745,7 @@
         <v>INSERT INTO `song` (`id`, `song_name`, `artist_id`, `album_id`, `song_description`, `song_length`, `song_url`) VALUES (NULL,'Caramelo (Remix)','2','1','','0','https://www.parkwaycleanersorl.com/music/ozuna/enoc/Caramelo%(Remix).mp3');</v>
       </c>
     </row>
-    <row r="30" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B30" t="str">
         <f t="shared" si="0"/>
         <v>https://www.parkwaycleanersorl.com/music/ozuna/enoc/Caramelo.mp3</v>
@@ -1768,7 +1777,7 @@
         <v>INSERT INTO `song` (`id`, `song_name`, `artist_id`, `album_id`, `song_description`, `song_length`, `song_url`) VALUES (NULL,'Caramelo','2','1','','0','https://www.parkwaycleanersorl.com/music/ozuna/enoc/Caramelo.mp3');</v>
       </c>
     </row>
-    <row r="31" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B31" t="str">
         <f t="shared" si="0"/>
         <v>https://www.parkwaycleanersorl.com/music/ozuna/enoc/Del Mar.mp3</v>
@@ -1800,7 +1809,7 @@
         <v>INSERT INTO `song` (`id`, `song_name`, `artist_id`, `album_id`, `song_description`, `song_length`, `song_url`) VALUES (NULL,'Del Mar','2','1','','0','https://www.parkwaycleanersorl.com/music/ozuna/enoc/Del%Mar.mp3');</v>
       </c>
     </row>
-    <row r="32" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B32" t="str">
         <f t="shared" si="0"/>
         <v>https://www.parkwaycleanersorl.com/music/ozuna/enoc/Enemigos Ocultos.mp3</v>
@@ -1832,7 +1841,7 @@
         <v>INSERT INTO `song` (`id`, `song_name`, `artist_id`, `album_id`, `song_description`, `song_length`, `song_url`) VALUES (NULL,'Enemigos Ocultos','2','1','','0','https://www.parkwaycleanersorl.com/music/ozuna/enoc/Enemigos%Ocultos.mp3');</v>
       </c>
     </row>
-    <row r="33" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B33" t="str">
         <f t="shared" si="0"/>
         <v>https://www.parkwaycleanersorl.com/music/ozuna/enoc/Mala.mp3</v>
@@ -1864,7 +1873,7 @@
         <v>INSERT INTO `song` (`id`, `song_name`, `artist_id`, `album_id`, `song_description`, `song_length`, `song_url`) VALUES (NULL,'Mala','2','1','','0','https://www.parkwaycleanersorl.com/music/ozuna/enoc/Mala.mp3');</v>
       </c>
     </row>
-    <row r="34" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B34" t="str">
         <f t="shared" si="0"/>
         <v>https://www.parkwaycleanersorl.com/music/ozuna/enoc/No Se Da Cuenta.mp3</v>
@@ -1896,7 +1905,7 @@
         <v>INSERT INTO `song` (`id`, `song_name`, `artist_id`, `album_id`, `song_description`, `song_length`, `song_url`) VALUES (NULL,'No Se Da Cuenta','2','1','','0','https://www.parkwaycleanersorl.com/music/ozuna/enoc/No%Se%Da%Cuenta.mp3');</v>
       </c>
     </row>
-    <row r="35" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B35" t="str">
         <f t="shared" si="0"/>
         <v>https://www.parkwaycleanersorl.com/music/ozuna/enoc/Que Tú Esperas.mp3</v>
@@ -1928,7 +1937,7 @@
         <v>INSERT INTO `song` (`id`, `song_name`, `artist_id`, `album_id`, `song_description`, `song_length`, `song_url`) VALUES (NULL,'Que Tú Esperas','2','1','','0','https://www.parkwaycleanersorl.com/music/ozuna/enoc/Que%Tú%Esperas.mp3');</v>
       </c>
     </row>
-    <row r="36" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B36" t="str">
         <f t="shared" si="0"/>
         <v>https://www.parkwaycleanersorl.com/music/ozuna/enoc/Sincero.mp3</v>
@@ -1960,7 +1969,7 @@
         <v>INSERT INTO `song` (`id`, `song_name`, `artist_id`, `album_id`, `song_description`, `song_length`, `song_url`) VALUES (NULL,'Sincero','2','1','','0','https://www.parkwaycleanersorl.com/music/ozuna/enoc/Sincero.mp3');</v>
       </c>
     </row>
-    <row r="37" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B37" t="str">
         <f t="shared" si="0"/>
         <v>https://www.parkwaycleanersorl.com/music/ozuna/enoc/Un Get.mp3</v>
@@ -1992,7 +2001,7 @@
         <v>INSERT INTO `song` (`id`, `song_name`, `artist_id`, `album_id`, `song_description`, `song_length`, `song_url`) VALUES (NULL,'Un Get','2','1','','0','https://www.parkwaycleanersorl.com/music/ozuna/enoc/Un%Get.mp3');</v>
       </c>
     </row>
-    <row r="38" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B38" t="str">
         <f t="shared" si="0"/>
         <v>https://www.parkwaycleanersorl.com/music/ozuna/enoc/Una Locura.mp3</v>
@@ -2023,7 +2032,7 @@
         <v>INSERT INTO `song` (`id`, `song_name`, `artist_id`, `album_id`, `song_description`, `song_length`, `song_url`) VALUES (NULL,'Una Locura','2','1','','0','https://www.parkwaycleanersorl.com/music/ozuna/enoc/Una%Locura.mp3');</v>
       </c>
     </row>
-    <row r="39" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B39" t="str">
         <f t="shared" si="0"/>
         <v>https://www.parkwaycleanersorl.com/music/ozuna/odisea/Ozuna - Carita de Ángel (Audio Oficial) - Odisea.mp3</v>
@@ -2055,7 +2064,7 @@
         <v>INSERT INTO `song` (`id`, `song_name`, `artist_id`, `album_id`, `song_description`, `song_length`, `song_url`) VALUES (NULL,'Carita De Ángel','2','3','','0','https://www.parkwaycleanersorl.com/music/ozuna/odisea/Ozuna%-%Carita%de%Ángel%(Audio%Oficial)%-%Odisea.mp3');</v>
       </c>
     </row>
-    <row r="40" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B40" t="str">
         <f t="shared" si="0"/>
         <v>https://www.parkwaycleanersorl.com/music/ozuna/odisea/Ozuna - Dile Que Tu Me Quieres (Video Oficial) - Odisea.mp3</v>
@@ -2087,7 +2096,7 @@
         <v>INSERT INTO `song` (`id`, `song_name`, `artist_id`, `album_id`, `song_description`, `song_length`, `song_url`) VALUES (NULL,'Dile Que Tu Me Quieres','2','3','','0','https://www.parkwaycleanersorl.com/music/ozuna/odisea/Ozuna%-%Dile%Que%Tu%Me%Quieres%(Video%Oficial)%-%Odisea.mp3');</v>
       </c>
     </row>
-    <row r="41" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B41" t="str">
         <f t="shared" si="0"/>
         <v>https://www.parkwaycleanersorl.com/music/ozuna/odisea/Ozuna - El Farsante (Audio Oficial) - Odisea.mp3</v>
@@ -2119,7 +2128,7 @@
         <v>INSERT INTO `song` (`id`, `song_name`, `artist_id`, `album_id`, `song_description`, `song_length`, `song_url`) VALUES (NULL,'El Farsante','2','3','','0','https://www.parkwaycleanersorl.com/music/ozuna/odisea/Ozuna%-%El%Farsante%(Audio%Oficial)%-%Odisea.mp3');</v>
       </c>
     </row>
-    <row r="42" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B42" t="str">
         <f t="shared" si="0"/>
         <v>https://www.parkwaycleanersorl.com/music/ozuna/odisea/Ozuna - No Quiere Enamorarse (Official Lyric Video).mp3</v>
@@ -2151,7 +2160,7 @@
         <v>INSERT INTO `song` (`id`, `song_name`, `artist_id`, `album_id`, `song_description`, `song_length`, `song_url`) VALUES (NULL,'No Quiere Enamorarse','2','3','','0','https://www.parkwaycleanersorl.com/music/ozuna/odisea/Ozuna%-%No%Quiere%Enamorarse%(Official%Lyric%Video).mp3');</v>
       </c>
     </row>
-    <row r="43" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B43" t="str">
         <f t="shared" si="0"/>
         <v>https://www.parkwaycleanersorl.com/music/ozuna/odisea/Ozuna - Noches de Aventura (Audio Oficial) - Odisea.mp3</v>
@@ -2183,7 +2192,7 @@
         <v>INSERT INTO `song` (`id`, `song_name`, `artist_id`, `album_id`, `song_description`, `song_length`, `song_url`) VALUES (NULL,'Noches De Aventura','2','3','','0','https://www.parkwaycleanersorl.com/music/ozuna/odisea/Ozuna%-%Noches%de%Aventura%(Audio%Oficial)%-%Odisea.mp3');</v>
       </c>
     </row>
-    <row r="44" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B44" t="str">
         <f t="shared" si="0"/>
         <v>https://www.parkwaycleanersorl.com/music/ozuna/odisea/Ozuna - Odisea (Audio Oficial) - Odisea.mp3</v>
@@ -2215,7 +2224,7 @@
         <v>INSERT INTO `song` (`id`, `song_name`, `artist_id`, `album_id`, `song_description`, `song_length`, `song_url`) VALUES (NULL,'Odisea','2','3','','0','https://www.parkwaycleanersorl.com/music/ozuna/odisea/Ozuna%-%Odisea%(Audio%Oficial)%-%Odisea.mp3');</v>
       </c>
     </row>
-    <row r="45" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B45" t="str">
         <f t="shared" si="0"/>
         <v>https://www.parkwaycleanersorl.com/music/ozuna/odisea/Ozuna - Se Preparó (Video Oficial) - Odisea.mp3</v>
@@ -2247,7 +2256,7 @@
         <v>INSERT INTO `song` (`id`, `song_name`, `artist_id`, `album_id`, `song_description`, `song_length`, `song_url`) VALUES (NULL,'Se Preparó','2','3','','0','https://www.parkwaycleanersorl.com/music/ozuna/odisea/Ozuna%-%Se%Preparó%(Video%Oficial)%-%Odisea.mp3');</v>
       </c>
     </row>
-    <row r="46" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B46" t="str">
         <f t="shared" si="0"/>
         <v>https://www.parkwaycleanersorl.com/music/ozuna/odisea/Ozuna - Si Tu Marido No Te Quiere (Official Lyric Video).mp3</v>
@@ -2279,7 +2288,7 @@
         <v>INSERT INTO `song` (`id`, `song_name`, `artist_id`, `album_id`, `song_description`, `song_length`, `song_url`) VALUES (NULL,'Si Tu Marido No Te Quiere','2','3','','0','https://www.parkwaycleanersorl.com/music/ozuna/odisea/Ozuna%-%Si%Tu%Marido%No%Te%Quiere%(Official%Lyric%Video).mp3');</v>
       </c>
     </row>
-    <row r="47" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B47" t="str">
         <f t="shared" si="0"/>
         <v>https://www.parkwaycleanersorl.com/music/ozuna/odisea/Ozuna - Síguelo Bailando (Video Oficial).mp3</v>
@@ -2311,7 +2320,7 @@
         <v>INSERT INTO `song` (`id`, `song_name`, `artist_id`, `album_id`, `song_description`, `song_length`, `song_url`) VALUES (NULL,'Síguelo Bailando','2','3','','0','https://www.parkwaycleanersorl.com/music/ozuna/odisea/Ozuna%-%Síguelo%Bailando%(Video%Oficial).mp3');</v>
       </c>
     </row>
-    <row r="48" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B48" t="str">
         <f t="shared" si="0"/>
         <v>https://www.parkwaycleanersorl.com/music/ozuna/odisea/Ozuna - Tu Foto (Video Oficial) - Odisea.mp3</v>
@@ -2343,7 +2352,7 @@
         <v>INSERT INTO `song` (`id`, `song_name`, `artist_id`, `album_id`, `song_description`, `song_length`, `song_url`) VALUES (NULL,'Tu Foto','2','3','','0','https://www.parkwaycleanersorl.com/music/ozuna/odisea/Ozuna%-%Tu%Foto%(Video%Oficial)%-%Odisea.mp3');</v>
       </c>
     </row>
-    <row r="49" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B49" t="str">
         <f t="shared" si="0"/>
         <v>https://www.parkwaycleanersorl.com/music/ozuna/odisea/Ozuna - Una Flor (Video Oficial) - Odisea.mp3</v>
@@ -2375,7 +2384,7 @@
         <v>INSERT INTO `song` (`id`, `song_name`, `artist_id`, `album_id`, `song_description`, `song_length`, `song_url`) VALUES (NULL,'Una Flor','2','3','','0','https://www.parkwaycleanersorl.com/music/ozuna/odisea/Ozuna%-%Una%Flor%(Video%Oficial)%-%Odisea.mp3');</v>
       </c>
     </row>
-    <row r="50" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B50" t="str">
         <f t="shared" si="0"/>
         <v>https://www.parkwaycleanersorl.com/music/ozuna/odisea/Ozuna feat. J Balvin - Quiero Repetir (Audio Oficial) - Odisea.mp3</v>
@@ -2407,7 +2416,7 @@
         <v>INSERT INTO `song` (`id`, `song_name`, `artist_id`, `album_id`, `song_description`, `song_length`, `song_url`) VALUES (NULL,'Quiero Repetir','2','3','','0','https://www.parkwaycleanersorl.com/music/ozuna/odisea/Ozuna%feat.%J%Balvin%-%Quiero%Repetir%(Audio%Oficial)%-%Odisea.mp3');</v>
       </c>
     </row>
-    <row r="51" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B51" t="str">
         <f t="shared" si="0"/>
         <v>https://www.parkwaycleanersorl.com/music/ozuna/odisea/Ozuna feat. Nicky Jam - Cumpleaños (Audio Oficial) - Odisea.mp3</v>
@@ -2439,7 +2448,7 @@
         <v>INSERT INTO `song` (`id`, `song_name`, `artist_id`, `album_id`, `song_description`, `song_length`, `song_url`) VALUES (NULL,'Cumpleaños','2','3','','0','https://www.parkwaycleanersorl.com/music/ozuna/odisea/Ozuna%feat.%Nicky%Jam%-%Cumpleaños%(Audio%Oficial)%-%Odisea.mp3');</v>
       </c>
     </row>
-    <row r="52" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B52" t="str">
         <f t="shared" si="0"/>
         <v>https://www.parkwaycleanersorl.com/music/ozuna/odisea/Ozuna feat. Zion &amp; Lennox - Egoísta (Audio Oficial) - Odisea.mp3</v>
@@ -2471,7 +2480,7 @@
         <v>INSERT INTO `song` (`id`, `song_name`, `artist_id`, `album_id`, `song_description`, `song_length`, `song_url`) VALUES (NULL,'Egoísta','2','3','','0','https://www.parkwaycleanersorl.com/music/ozuna/odisea/Ozuna%feat.%Zion%&amp;%Lennox%-%Egoísta%(Audio%Oficial)%-%Odisea.mp3');</v>
       </c>
     </row>
-    <row r="53" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B53" t="str">
         <f t="shared" si="0"/>
         <v>https://www.parkwaycleanersorl.com/music/ozuna/odisea/Ozuna FT Anuel AA - Bebe (Lyric Video) - Odisea.mp3</v>
@@ -2502,88 +2511,88 @@
         <v>INSERT INTO `song` (`id`, `song_name`, `artist_id`, `album_id`, `song_description`, `song_length`, `song_url`) VALUES (NULL,'Bebe','2','3','','0','https://www.parkwaycleanersorl.com/music/ozuna/odisea/Ozuna%FT%Anuel%AA%-%Bebe%(Lyric%Video)%-%Odisea.mp3');</v>
       </c>
     </row>
-    <row r="54" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D54" s="4"/>
     </row>
-    <row r="55" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D55" s="4"/>
     </row>
-    <row r="56" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D56" s="4"/>
     </row>
-    <row r="57" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D57" s="4"/>
     </row>
-    <row r="58" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D58" s="4"/>
     </row>
-    <row r="59" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D59" s="4"/>
     </row>
-    <row r="60" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D60" s="4"/>
     </row>
-    <row r="61" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D61" s="4"/>
     </row>
-    <row r="62" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D62" s="4"/>
     </row>
-    <row r="63" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D63" s="4"/>
     </row>
-    <row r="64" spans="2:11" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:11" x14ac:dyDescent="0.25">
       <c r="D64" s="4"/>
     </row>
-    <row r="65" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D65" s="4"/>
     </row>
-    <row r="66" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D66" s="4"/>
     </row>
-    <row r="67" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D67" s="4"/>
     </row>
-    <row r="68" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D68" s="4"/>
     </row>
-    <row r="69" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D69" s="4"/>
     </row>
-    <row r="70" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D70" s="4"/>
     </row>
-    <row r="71" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D71" s="4"/>
     </row>
-    <row r="72" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="72" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D72" s="4"/>
     </row>
-    <row r="73" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="73" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D73" s="4"/>
     </row>
-    <row r="74" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="74" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D74" s="4"/>
     </row>
-    <row r="75" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="75" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D75" s="4"/>
     </row>
-    <row r="76" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="76" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D76" s="4"/>
     </row>
-    <row r="77" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="77" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D77" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C4" r:id="rId1"/>
-    <hyperlink ref="C15" r:id="rId2"/>
-    <hyperlink ref="C5:C14" r:id="rId3" display="https://www.parkwaycleanersorl.com/music/daddy-yankee/king-daddy/"/>
-    <hyperlink ref="C16:C28" r:id="rId4" display="https://www.parkwaycleanersorl.com/music/maria-becerra/animal/"/>
-    <hyperlink ref="C29" r:id="rId5"/>
-    <hyperlink ref="C30:C38" r:id="rId6" display="https://www.parkwaycleanersorl.com/music/ozuna/enoc/"/>
-    <hyperlink ref="C39" r:id="rId7"/>
-    <hyperlink ref="C40:C53" r:id="rId8" display="https://www.parkwaycleanersorl.com/music/ozuna/odisea/"/>
+    <hyperlink ref="C4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="C15" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="C5:C14" r:id="rId3" display="https://www.parkwaycleanersorl.com/music/daddy-yankee/king-daddy/" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="C16:C28" r:id="rId4" display="https://www.parkwaycleanersorl.com/music/maria-becerra/animal/" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="C29" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="C30:C38" r:id="rId6" display="https://www.parkwaycleanersorl.com/music/ozuna/enoc/" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="C39" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="C40:C53" r:id="rId8" display="https://www.parkwaycleanersorl.com/music/ozuna/odisea/" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId9"/>

</xml_diff>